<commit_message>
Function for building query for ISBNs
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -50,13 +50,13 @@
     <t>12346567 3723</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Tittel</t>
+  </si>
+  <si>
+    <t>Forlag</t>
   </si>
   <si>
     <t>9788202788629</t>
@@ -123,9 +123,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="2" totalsRowFunction="none"/>
-    <tableColumn id="3" name="3" totalsRowFunction="none"/>
+    <tableColumn id="1" name="ISBN" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Tittel" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Forlag" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Write result from promus to new worksheet
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>9788249527496</t>
   </si>
@@ -59,7 +59,28 @@
     <t>Forlag</t>
   </si>
   <si>
-    <t>9788202788629</t>
+    <t>Blokka</t>
+  </si>
+  <si>
+    <t>Aschehoug</t>
+  </si>
+  <si>
+    <t>Vinter i Applemore</t>
+  </si>
+  <si>
+    <t>Gyldendal</t>
+  </si>
+  <si>
+    <t>Alle utlendinger har lukka gardiner</t>
+  </si>
+  <si>
+    <t>Lydbokforlaget</t>
+  </si>
+  <si>
+    <t>Jeg plystrer i den mørke vinden</t>
+  </si>
+  <si>
+    <t>Oktober</t>
   </si>
 </sst>
 </file>
@@ -116,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="MyTable" displayName="MyTable" ref="A1:C8" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:C8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="MyTable" displayName="MyTable" ref="A1:C5" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -431,7 +452,7 @@
   <dimension ref="A2:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
@@ -455,9 +476,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
@@ -505,7 +523,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="20"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -521,79 +539,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added descriptive logging to script. Created a .cmd file for running script
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64EF912-C17B-4B2D-83EC-0A58ABC46115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="12645"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Result" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>9788249527496</t>
   </si>
@@ -48,52 +48,19 @@
   </si>
   <si>
     <t>12346567 3723</t>
-  </si>
-  <si>
-    <t>ISBN</t>
-  </si>
-  <si>
-    <t>Tittel</t>
-  </si>
-  <si>
-    <t>Forlag</t>
-  </si>
-  <si>
-    <t>Blokka</t>
-  </si>
-  <si>
-    <t>Aschehoug</t>
-  </si>
-  <si>
-    <t>Vinter i Applemore</t>
-  </si>
-  <si>
-    <t>Gyldendal</t>
-  </si>
-  <si>
-    <t>Alle utlendinger har lukka gardiner</t>
-  </si>
-  <si>
-    <t>Lydbokforlaget</t>
-  </si>
-  <si>
-    <t>Jeg plystrer i den mørke vinden</t>
-  </si>
-  <si>
-    <t>Oktober</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,22 +101,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="MyTable" displayName="MyTable" ref="A1:C5" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:C5">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="1" name="ISBN" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Tittel" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Forlag" totalsRowFunction="none"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,14 +399,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
@@ -519,73 +470,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="20"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
npm install when running script
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64EF912-C17B-4B2D-83EC-0A58ABC46115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Result" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>9788249527496</t>
   </si>
@@ -48,19 +48,52 @@
   </si>
   <si>
     <t>12346567 3723</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Tittel</t>
+  </si>
+  <si>
+    <t>Forlag</t>
+  </si>
+  <si>
+    <t>Blokka</t>
+  </si>
+  <si>
+    <t>Aschehoug</t>
+  </si>
+  <si>
+    <t>Vinter i Applemore</t>
+  </si>
+  <si>
+    <t>Gyldendal</t>
+  </si>
+  <si>
+    <t>Alle utlendinger har lukka gardiner</t>
+  </si>
+  <si>
+    <t>Lydbokforlaget</t>
+  </si>
+  <si>
+    <t>Jeg plystrer i den mørke vinden</t>
+  </si>
+  <si>
+    <t>Forlaget Oktober</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,6 +134,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="MyTable" displayName="MyTable" ref="A1:C5" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:C5">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="ISBN" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Tittel" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Forlag" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,14 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
@@ -470,4 +519,73 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="20"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>